<commit_message>
update data upah harian pcc
</commit_message>
<xml_diff>
--- a/Rekap Harian PCC.xlsx
+++ b/Rekap Harian PCC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\ssi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C732A7-B12A-48F6-8FFD-75B94032DBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B0B368-9F23-42D2-85EC-9D27E3FD3401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{075B4635-85EB-4CA7-B4E8-4A8915099A4D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{075B4635-85EB-4CA7-B4E8-4A8915099A4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Harian 23.001" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="20">
   <si>
     <t>Periode Awal</t>
   </si>
@@ -240,691 +240,7 @@
     <cellStyle name="Normal 3" xfId="8" xr:uid="{0CBCE864-16BA-4B56-BF69-C5A4E9F4DF51}"/>
     <cellStyle name="Normal 4" xfId="2" xr:uid="{D37E4E15-39E3-4294-80AE-BB1DDB9D79EC}"/>
   </cellStyles>
-  <dxfs count="130">
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="33" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <border>
         <bottom style="thin">
@@ -3341,19 +2657,19 @@
     <dataField name="Sum of Nominal" fld="3" baseField="0" baseItem="0" numFmtId="41"/>
   </dataFields>
   <formats count="25">
-    <format dxfId="75">
+    <format dxfId="24">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="23">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="22">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="21">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="20">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="5" count="5">
@@ -3366,10 +2682,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -3381,7 +2697,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="2">
@@ -3394,7 +2710,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="83">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="5">
@@ -3410,7 +2726,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="3">
@@ -3424,7 +2740,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="2">
@@ -3437,7 +2753,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3452,7 +2768,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3468,7 +2784,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3484,7 +2800,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="89">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3500,7 +2816,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3516,7 +2832,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3532,7 +2848,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3548,7 +2864,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="93">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3564,7 +2880,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="94">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3580,7 +2896,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="95">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3596,7 +2912,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3615,7 +2931,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3635,7 +2951,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="0" count="1" selected="0">
@@ -3648,7 +2964,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="99">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -3665,13 +2981,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D5433F41-2172-40BD-B7A3-B4FCC4F3D6BF}" name="Table1" displayName="Table1" ref="B4:E41" totalsRowShown="0" headerRowDxfId="129">
-  <autoFilter ref="B4:E41" xr:uid="{D5433F41-2172-40BD-B7A3-B4FCC4F3D6BF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D5433F41-2172-40BD-B7A3-B4FCC4F3D6BF}" name="Table1" displayName="Table1" ref="B4:E79" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="B4:E79" xr:uid="{D5433F41-2172-40BD-B7A3-B4FCC4F3D6BF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{47374319-4F6B-4451-979D-6FB7A4961B6F}" name="Periode Awal" dataDxfId="128"/>
-    <tableColumn id="2" xr3:uid="{00563768-5306-4A9F-886D-F8192DE5F543}" name="Peride Akhir" dataDxfId="127"/>
-    <tableColumn id="3" xr3:uid="{1FED64DD-A9B5-4DD7-8394-6F5608CF3D09}" name="Deskripsi" dataDxfId="126"/>
-    <tableColumn id="4" xr3:uid="{50964661-1B7E-49EA-BB6A-8DB4BBE0A90F}" name="Nominal" dataDxfId="125" dataCellStyle="Comma [0]"/>
+    <tableColumn id="1" xr3:uid="{47374319-4F6B-4451-979D-6FB7A4961B6F}" name="Periode Awal" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00563768-5306-4A9F-886D-F8192DE5F543}" name="Peride Akhir" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{1FED64DD-A9B5-4DD7-8394-6F5608CF3D09}" name="Deskripsi" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{50964661-1B7E-49EA-BB6A-8DB4BBE0A90F}" name="Nominal" dataDxfId="25" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3974,10 +3290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D8F4B2-0B58-4C37-B383-E7721AC98F8C}">
-  <dimension ref="B2:E41"/>
+  <dimension ref="B2:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M72" sqref="M72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3985,8 +3301,8 @@
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" style="3" customWidth="1"/>
     <col min="3" max="3" width="13.109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
@@ -4527,6 +3843,538 @@
       </c>
       <c r="E41" s="5">
         <v>41306400</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
+        <v>45116</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45129</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="5">
+        <v>24225400</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" s="2">
+        <v>45130</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45143</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="5">
+        <v>22271200</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
+        <v>45144</v>
+      </c>
+      <c r="C44" s="2">
+        <v>45157</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="5">
+        <v>19299400</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B45" s="2">
+        <v>45158</v>
+      </c>
+      <c r="C45" s="2">
+        <v>45171</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="5">
+        <v>21150000</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B46" s="2">
+        <v>45172</v>
+      </c>
+      <c r="C46" s="2">
+        <v>45185</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="5">
+        <v>18925200</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B47" s="2">
+        <v>45186</v>
+      </c>
+      <c r="C47" s="2">
+        <v>45199</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="5">
+        <v>19388400</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B48" s="2">
+        <v>45200</v>
+      </c>
+      <c r="C48" s="2">
+        <v>45213</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E48" s="5">
+        <v>21710200</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B49" s="2">
+        <v>45214</v>
+      </c>
+      <c r="C49" s="2">
+        <v>45227</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="5">
+        <v>21382400</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="2">
+        <v>45228</v>
+      </c>
+      <c r="C50" s="2">
+        <v>45241</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="5">
+        <v>20081200</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" s="2">
+        <v>45116</v>
+      </c>
+      <c r="C51" s="2">
+        <v>45129</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" s="5">
+        <v>86520000</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="2">
+        <v>45130</v>
+      </c>
+      <c r="C52" s="2">
+        <v>45143</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="5">
+        <v>73997450</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="2">
+        <v>45144</v>
+      </c>
+      <c r="C53" s="2">
+        <v>45157</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="5">
+        <v>58252125</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="2">
+        <v>45158</v>
+      </c>
+      <c r="C54" s="2">
+        <v>45171</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="5">
+        <v>46882025</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="2">
+        <v>45172</v>
+      </c>
+      <c r="C55" s="2">
+        <v>45185</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="5">
+        <v>49916700</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="2">
+        <v>45186</v>
+      </c>
+      <c r="C56" s="2">
+        <v>45199</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="5">
+        <v>49696150</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57" s="2">
+        <v>45200</v>
+      </c>
+      <c r="C57" s="2">
+        <v>45213</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" s="5">
+        <v>58555500</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="2">
+        <v>45214</v>
+      </c>
+      <c r="C58" s="2">
+        <v>45227</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="5">
+        <v>58796775</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="2">
+        <v>45228</v>
+      </c>
+      <c r="C59" s="2">
+        <v>45241</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="5">
+        <v>44149525</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="2">
+        <v>45116</v>
+      </c>
+      <c r="C60" s="2">
+        <v>45129</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="5">
+        <v>54569450</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="2">
+        <v>45130</v>
+      </c>
+      <c r="C61" s="2">
+        <v>45143</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="5">
+        <v>77646975</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="2">
+        <v>45144</v>
+      </c>
+      <c r="C62" s="2">
+        <v>45157</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="5">
+        <v>88653300</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="2">
+        <v>45158</v>
+      </c>
+      <c r="C63" s="2">
+        <v>45171</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="5">
+        <v>85171075</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B64" s="2">
+        <v>45172</v>
+      </c>
+      <c r="C64" s="2">
+        <v>45185</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="5">
+        <v>80288925</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="2">
+        <v>45186</v>
+      </c>
+      <c r="C65" s="2">
+        <v>45199</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="5">
+        <v>86789650</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="2">
+        <v>45200</v>
+      </c>
+      <c r="C66" s="2">
+        <v>45213</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="5">
+        <v>80944575</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="2">
+        <v>45214</v>
+      </c>
+      <c r="C67" s="2">
+        <v>45227</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="5">
+        <v>78798550</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68" s="2">
+        <v>45228</v>
+      </c>
+      <c r="C68" s="2">
+        <v>45241</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="5">
+        <v>69366350</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B69" s="2">
+        <v>45116</v>
+      </c>
+      <c r="C69" s="2">
+        <v>45129</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="5">
+        <v>49793625</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B70" s="2">
+        <v>45130</v>
+      </c>
+      <c r="C70" s="2">
+        <v>45143</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="5">
+        <v>82821750</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B71" s="2">
+        <v>45144</v>
+      </c>
+      <c r="C71" s="2">
+        <v>45157</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E71" s="5">
+        <v>75367125</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B72" s="2">
+        <v>45158</v>
+      </c>
+      <c r="C72" s="2">
+        <v>45171</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E72" s="5">
+        <v>87264000</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B73" s="2">
+        <v>45172</v>
+      </c>
+      <c r="C73" s="2">
+        <v>45185</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E73" s="5">
+        <v>78678600</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" s="2">
+        <v>45186</v>
+      </c>
+      <c r="C74" s="2">
+        <v>45199</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="5">
+        <v>101533500</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B75" s="2">
+        <v>45200</v>
+      </c>
+      <c r="C75" s="2">
+        <v>45213</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="5">
+        <v>92418750</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B76" s="2">
+        <v>45214</v>
+      </c>
+      <c r="C76" s="2">
+        <v>45227</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="5">
+        <v>91655250</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B77" s="2">
+        <v>45228</v>
+      </c>
+      <c r="C77" s="2">
+        <v>45241</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="5">
+        <v>85588500</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B78" s="2">
+        <v>45116</v>
+      </c>
+      <c r="C78" s="2">
+        <v>45129</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="5">
+        <v>4377550</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="2">
+        <v>45116</v>
+      </c>
+      <c r="C79" s="2">
+        <v>45129</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" s="5">
+        <v>52166625</v>
       </c>
     </row>
   </sheetData>
@@ -4548,7 +4396,7 @@
   </sheetPr>
   <dimension ref="A3:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update data upah harian
</commit_message>
<xml_diff>
--- a/Rekap Harian PCC.xlsx
+++ b/Rekap Harian PCC.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15915" windowHeight="7815" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Harian 23.001" sheetId="1" r:id="rId1"/>
     <sheet name="Pivot Harian 23.001" sheetId="2" r:id="rId2"/>
     <sheet name="Gaji 23.001" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="55">
   <si>
     <t>Rekap Upah Harian [23.001] PCC</t>
   </si>
@@ -173,21 +174,33 @@
   <si>
     <t>Gaji Electrical Okt</t>
   </si>
+  <si>
+    <t>Costcode</t>
+  </si>
+  <si>
+    <t>Harian Semi Fitter, Rigger, Scaffolder lokal</t>
+  </si>
+  <si>
+    <t>Harian Fitter Pagar Laydown</t>
+  </si>
+  <si>
+    <t>Harian Helper Local</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_(* #,###.00_);_(* \(#,###.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="_(* #,###.00_);_(* \(#,###.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="181" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-_);_(@_)"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,49 +217,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -257,24 +231,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -283,20 +241,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,10 +255,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -323,14 +266,75 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -345,7 +349,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,9 +371,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -381,13 +387,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +435,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,13 +453,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,37 +495,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,13 +513,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,7 +555,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,66 +567,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -575,11 +581,65 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -603,22 +663,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,30 +673,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -684,198 +705,193 @@
   </borders>
   <cellStyleXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="181" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="181" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="181" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -884,9 +900,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -945,8 +958,8 @@
     <cellStyle name="Accent6" xfId="51" builtinId="49"/>
     <cellStyle name="40% - Accent6" xfId="52" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="53" builtinId="52"/>
-    <cellStyle name="Comma 2" xfId="54"/>
-    <cellStyle name="Comma [0] 2" xfId="55"/>
+    <cellStyle name="Comma [0] 2" xfId="54"/>
+    <cellStyle name="Comma 2" xfId="55"/>
     <cellStyle name="Excel Built-in Comma [0] 1" xfId="56"/>
     <cellStyle name="Normal 2 2" xfId="57"/>
   </cellStyles>
@@ -1156,7 +1169,7 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="181" formatCode="_(* #,###.00_);_(* \(#,###.00\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="180" formatCode="_(* #,###.00_);_(* \(#,###.00\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
@@ -1239,7 +1252,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Nominal" numFmtId="41">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1074350" maxValue="101533500" count="75">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="101533500" count="75">
         <n v="2453400"/>
         <n v="3261800"/>
         <n v="21684500"/>
@@ -4227,7 +4240,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:E79" totalsRowShown="0">
   <autoFilter ref="B4:E79"/>
-  <sortState ref="B5:E79">
+  <sortState ref="B4:E79">
     <sortCondition ref="B4"/>
   </sortState>
   <tableColumns count="4">
@@ -4513,25 +4526,25 @@
   <sheetPr/>
   <dimension ref="B2:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="13.8857142857143" style="15" customWidth="1"/>
-    <col min="3" max="3" width="13.1047619047619" style="15" customWidth="1"/>
-    <col min="4" max="4" width="36" style="16" customWidth="1"/>
-    <col min="5" max="5" width="12.4380952380952" style="17" customWidth="1"/>
+    <col min="2" max="2" width="13.8857142857143" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.1047619047619" style="4" customWidth="1"/>
+    <col min="4" max="4" width="36" style="15" customWidth="1"/>
+    <col min="5" max="5" width="12.4380952380952" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="6" t="s">
@@ -4543,1057 +4556,1057 @@
       <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="19">
+      <c r="B5" s="8">
         <v>44983</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="8">
         <v>44996</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>2453400</v>
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="19">
+      <c r="B6" s="8">
         <v>44997</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="8">
         <v>45010</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>3261800</v>
       </c>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="19">
+      <c r="B7" s="8">
         <v>44997</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="8">
         <v>45010</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>21684500</v>
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="19">
+      <c r="B8" s="8">
         <v>45011</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="8">
         <v>45024</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>8168600</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="19">
+      <c r="B9" s="8">
         <v>45011</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="8">
         <v>45024</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>25578000</v>
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="19">
+      <c r="B10" s="8">
         <v>45025</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="8">
         <v>45038</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>8789000</v>
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="19">
+      <c r="B11" s="8">
         <v>45025</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="8">
         <v>45038</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <v>28737725</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="19">
+      <c r="B12" s="8">
         <v>45030</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="8">
         <v>45073</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>38966625</v>
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="19">
+      <c r="B13" s="8">
         <v>45030</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="8">
         <v>45073</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>19806200</v>
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="19">
+      <c r="B14" s="8">
         <v>45032</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="8">
         <v>45045</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="16">
         <v>10078875</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="19">
+      <c r="B15" s="8">
         <v>45032</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="8">
         <v>45045</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="16">
         <v>13255000</v>
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="19">
+      <c r="B16" s="8">
         <v>45039</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="8">
         <v>45052</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="16">
         <v>13739000</v>
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="19">
+      <c r="B17" s="8">
         <v>45039</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="8">
         <v>45052</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="16">
         <v>42455475</v>
       </c>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="19">
+      <c r="B18" s="8">
         <v>45046</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="8">
         <v>45059</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="16">
         <v>36031125</v>
       </c>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="19">
+      <c r="B19" s="8">
         <v>45046</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="8">
         <v>45059</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="16">
         <v>25777000</v>
       </c>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="19">
+      <c r="B20" s="8">
         <v>45053</v>
       </c>
-      <c r="C20" s="19">
+      <c r="C20" s="8">
         <v>45066</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="16">
         <v>14653400</v>
       </c>
     </row>
     <row r="21" spans="2:5">
-      <c r="B21" s="19">
+      <c r="B21" s="8">
         <v>45053</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="8">
         <v>45066</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="16">
         <v>57089475</v>
       </c>
     </row>
     <row r="22" spans="2:5">
-      <c r="B22" s="19">
+      <c r="B22" s="8">
         <v>45067</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="8">
         <v>45073</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="16">
         <v>9406600</v>
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="19">
+      <c r="B23" s="8">
         <v>45067</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="8">
         <v>45073</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="16">
         <v>34994200</v>
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="19">
+      <c r="B24" s="8">
         <v>45074</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="8">
         <v>45087</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="16">
         <v>21443400</v>
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="19">
+      <c r="B25" s="8">
         <v>45074</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="8">
         <v>45087</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="16">
         <v>65945325</v>
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="19">
+      <c r="B26" s="8">
         <v>45074</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="8">
         <v>45087</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="16">
         <v>1074350</v>
       </c>
     </row>
     <row r="27" spans="2:5">
-      <c r="B27" s="19">
+      <c r="B27" s="8">
         <v>45074</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="8">
         <v>45087</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="17">
+      <c r="E27" s="16">
         <v>44873000</v>
       </c>
     </row>
     <row r="28" spans="2:5">
-      <c r="B28" s="19">
+      <c r="B28" s="8">
         <v>45074</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="8">
         <v>45087</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="16">
         <v>31695800</v>
       </c>
     </row>
     <row r="29" spans="2:5">
-      <c r="B29" s="19">
+      <c r="B29" s="8">
         <v>45088</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="8">
         <v>45101</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="17">
+      <c r="E29" s="16">
         <v>20764200</v>
       </c>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="19">
+      <c r="B30" s="8">
         <v>45088</v>
       </c>
-      <c r="C30" s="19">
+      <c r="C30" s="8">
         <v>45101</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="17">
+      <c r="E30" s="16">
         <v>78816700</v>
       </c>
     </row>
     <row r="31" spans="2:5">
-      <c r="B31" s="19">
+      <c r="B31" s="8">
         <v>45088</v>
       </c>
-      <c r="C31" s="19">
+      <c r="C31" s="8">
         <v>45101</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="16">
         <v>12074625</v>
       </c>
     </row>
     <row r="32" spans="2:5">
-      <c r="B32" s="19">
+      <c r="B32" s="8">
         <v>45088</v>
       </c>
-      <c r="C32" s="19">
+      <c r="C32" s="8">
         <v>45101</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="16">
         <v>7291700</v>
       </c>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="19">
+      <c r="B33" s="8">
         <v>45088</v>
       </c>
-      <c r="C33" s="19">
+      <c r="C33" s="8">
         <v>45101</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="17">
+      <c r="E33" s="16">
         <v>44717875</v>
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="19">
+      <c r="B34" s="8">
         <v>45088</v>
       </c>
-      <c r="C34" s="19">
+      <c r="C34" s="8">
         <v>45101</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="16">
         <v>36781150</v>
       </c>
     </row>
     <row r="35" spans="2:5">
-      <c r="B35" s="19">
+      <c r="B35" s="8">
         <v>45102</v>
       </c>
-      <c r="C35" s="19">
+      <c r="C35" s="8">
         <v>45115</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="17">
+      <c r="E35" s="16">
         <v>21082200</v>
       </c>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="19">
+      <c r="B36" s="8">
         <v>45102</v>
       </c>
-      <c r="C36" s="19">
+      <c r="C36" s="8">
         <v>45115</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="16">
         <v>75484800</v>
       </c>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="19">
+      <c r="B37" s="8">
         <v>45102</v>
       </c>
-      <c r="C37" s="19">
+      <c r="C37" s="8">
         <v>45115</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="17">
+      <c r="E37" s="16">
         <v>11700000</v>
       </c>
     </row>
     <row r="38" spans="2:5">
-      <c r="B38" s="19">
+      <c r="B38" s="8">
         <v>45102</v>
       </c>
-      <c r="C38" s="19">
+      <c r="C38" s="8">
         <v>45115</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="16">
         <v>36296250</v>
       </c>
     </row>
     <row r="39" spans="2:5">
-      <c r="B39" s="19">
+      <c r="B39" s="8">
         <v>45102</v>
       </c>
-      <c r="C39" s="19">
+      <c r="C39" s="8">
         <v>45115</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="16">
         <v>5410150</v>
       </c>
     </row>
     <row r="40" spans="2:5">
-      <c r="B40" s="19">
+      <c r="B40" s="8">
         <v>45102</v>
       </c>
-      <c r="C40" s="19">
+      <c r="C40" s="8">
         <v>45115</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E40" s="16">
         <v>43027875</v>
       </c>
     </row>
     <row r="41" spans="2:5">
-      <c r="B41" s="19">
+      <c r="B41" s="8">
         <v>45102</v>
       </c>
-      <c r="C41" s="19">
+      <c r="C41" s="8">
         <v>45115</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="16">
         <v>41306400</v>
       </c>
     </row>
     <row r="42" spans="2:5">
-      <c r="B42" s="19">
+      <c r="B42" s="8">
         <v>45116</v>
       </c>
-      <c r="C42" s="19">
+      <c r="C42" s="8">
         <v>45129</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="16">
         <v>24225400</v>
       </c>
     </row>
     <row r="43" spans="2:5">
-      <c r="B43" s="19">
+      <c r="B43" s="8">
         <v>45116</v>
       </c>
-      <c r="C43" s="19">
+      <c r="C43" s="8">
         <v>45129</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="17">
+      <c r="E43" s="16">
         <v>86520000</v>
       </c>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="19">
+      <c r="B44" s="8">
         <v>45116</v>
       </c>
-      <c r="C44" s="19">
+      <c r="C44" s="8">
         <v>45129</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="16">
         <v>54569450</v>
       </c>
     </row>
     <row r="45" spans="2:5">
-      <c r="B45" s="19">
+      <c r="B45" s="8">
         <v>45116</v>
       </c>
-      <c r="C45" s="19">
+      <c r="C45" s="8">
         <v>45129</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="17">
+      <c r="E45" s="16">
         <v>49793625</v>
       </c>
     </row>
     <row r="46" spans="2:5">
-      <c r="B46" s="19">
+      <c r="B46" s="8">
         <v>45116</v>
       </c>
-      <c r="C46" s="19">
+      <c r="C46" s="8">
         <v>45129</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="17">
+      <c r="E46" s="16">
         <v>4377550</v>
       </c>
     </row>
     <row r="47" spans="2:5">
-      <c r="B47" s="19">
+      <c r="B47" s="8">
         <v>45116</v>
       </c>
-      <c r="C47" s="19">
+      <c r="C47" s="8">
         <v>45129</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E47" s="17">
+      <c r="E47" s="16">
         <v>52166625</v>
       </c>
     </row>
     <row r="48" spans="2:5">
-      <c r="B48" s="19">
+      <c r="B48" s="8">
         <v>45130</v>
       </c>
-      <c r="C48" s="19">
+      <c r="C48" s="8">
         <v>45143</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E48" s="17">
+      <c r="E48" s="16">
         <v>22271200</v>
       </c>
     </row>
     <row r="49" spans="2:5">
-      <c r="B49" s="19">
+      <c r="B49" s="8">
         <v>45130</v>
       </c>
-      <c r="C49" s="19">
+      <c r="C49" s="8">
         <v>45143</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="17">
+      <c r="E49" s="16">
         <v>73997450</v>
       </c>
     </row>
     <row r="50" spans="2:5">
-      <c r="B50" s="19">
+      <c r="B50" s="8">
         <v>45130</v>
       </c>
-      <c r="C50" s="19">
+      <c r="C50" s="8">
         <v>45143</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E50" s="17">
+      <c r="E50" s="16">
         <v>77646975</v>
       </c>
     </row>
     <row r="51" spans="2:5">
-      <c r="B51" s="19">
+      <c r="B51" s="8">
         <v>45130</v>
       </c>
-      <c r="C51" s="19">
+      <c r="C51" s="8">
         <v>45143</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E51" s="17">
+      <c r="E51" s="16">
         <v>82821750</v>
       </c>
     </row>
     <row r="52" spans="2:5">
-      <c r="B52" s="19">
+      <c r="B52" s="8">
         <v>45144</v>
       </c>
-      <c r="C52" s="19">
+      <c r="C52" s="8">
         <v>45157</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E52" s="17">
+      <c r="E52" s="16">
         <v>19299400</v>
       </c>
     </row>
     <row r="53" spans="2:5">
-      <c r="B53" s="19">
+      <c r="B53" s="8">
         <v>45144</v>
       </c>
-      <c r="C53" s="19">
+      <c r="C53" s="8">
         <v>45157</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="17">
+      <c r="E53" s="16">
         <v>58252125</v>
       </c>
     </row>
     <row r="54" spans="2:5">
-      <c r="B54" s="19">
+      <c r="B54" s="8">
         <v>45144</v>
       </c>
-      <c r="C54" s="19">
+      <c r="C54" s="8">
         <v>45157</v>
       </c>
-      <c r="D54" s="16" t="s">
+      <c r="D54" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="17">
+      <c r="E54" s="16">
         <v>88653300</v>
       </c>
     </row>
     <row r="55" spans="2:5">
-      <c r="B55" s="19">
+      <c r="B55" s="8">
         <v>45144</v>
       </c>
-      <c r="C55" s="19">
+      <c r="C55" s="8">
         <v>45157</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="17">
+      <c r="E55" s="16">
         <v>75367125</v>
       </c>
     </row>
     <row r="56" spans="2:5">
-      <c r="B56" s="19">
+      <c r="B56" s="8">
         <v>45158</v>
       </c>
-      <c r="C56" s="19">
+      <c r="C56" s="8">
         <v>45171</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E56" s="17">
+      <c r="E56" s="16">
         <v>21150000</v>
       </c>
     </row>
     <row r="57" spans="2:5">
-      <c r="B57" s="19">
+      <c r="B57" s="8">
         <v>45158</v>
       </c>
-      <c r="C57" s="19">
+      <c r="C57" s="8">
         <v>45171</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E57" s="17">
+      <c r="E57" s="16">
         <v>46882025</v>
       </c>
     </row>
     <row r="58" spans="2:5">
-      <c r="B58" s="19">
+      <c r="B58" s="8">
         <v>45158</v>
       </c>
-      <c r="C58" s="19">
+      <c r="C58" s="8">
         <v>45171</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="17">
+      <c r="E58" s="16">
         <v>85171075</v>
       </c>
     </row>
     <row r="59" spans="2:5">
-      <c r="B59" s="19">
+      <c r="B59" s="8">
         <v>45158</v>
       </c>
-      <c r="C59" s="19">
+      <c r="C59" s="8">
         <v>45171</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E59" s="17">
+      <c r="E59" s="16">
         <v>87264000</v>
       </c>
     </row>
     <row r="60" spans="2:5">
-      <c r="B60" s="19">
+      <c r="B60" s="8">
         <v>45172</v>
       </c>
-      <c r="C60" s="19">
+      <c r="C60" s="8">
         <v>45185</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E60" s="17">
+      <c r="E60" s="16">
         <v>18925200</v>
       </c>
     </row>
     <row r="61" spans="2:5">
-      <c r="B61" s="19">
+      <c r="B61" s="8">
         <v>45172</v>
       </c>
-      <c r="C61" s="19">
+      <c r="C61" s="8">
         <v>45185</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E61" s="17">
+      <c r="E61" s="16">
         <v>49916700</v>
       </c>
     </row>
     <row r="62" spans="2:5">
-      <c r="B62" s="19">
+      <c r="B62" s="8">
         <v>45172</v>
       </c>
-      <c r="C62" s="19">
+      <c r="C62" s="8">
         <v>45185</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D62" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E62" s="17">
+      <c r="E62" s="16">
         <v>80288925</v>
       </c>
     </row>
     <row r="63" spans="2:5">
-      <c r="B63" s="19">
+      <c r="B63" s="8">
         <v>45172</v>
       </c>
-      <c r="C63" s="19">
+      <c r="C63" s="8">
         <v>45185</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E63" s="17">
+      <c r="E63" s="16">
         <v>78678600</v>
       </c>
     </row>
     <row r="64" spans="2:5">
-      <c r="B64" s="19">
+      <c r="B64" s="8">
         <v>45186</v>
       </c>
-      <c r="C64" s="19">
+      <c r="C64" s="8">
         <v>45199</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="17">
+      <c r="E64" s="16">
         <v>19388400</v>
       </c>
     </row>
     <row r="65" spans="2:5">
-      <c r="B65" s="19">
+      <c r="B65" s="8">
         <v>45186</v>
       </c>
-      <c r="C65" s="19">
+      <c r="C65" s="8">
         <v>45199</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E65" s="17">
+      <c r="E65" s="16">
         <v>49696150</v>
       </c>
     </row>
     <row r="66" spans="2:5">
-      <c r="B66" s="19">
+      <c r="B66" s="8">
         <v>45186</v>
       </c>
-      <c r="C66" s="19">
+      <c r="C66" s="8">
         <v>45199</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D66" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E66" s="17">
+      <c r="E66" s="16">
         <v>86789650</v>
       </c>
     </row>
     <row r="67" spans="2:5">
-      <c r="B67" s="19">
+      <c r="B67" s="8">
         <v>45186</v>
       </c>
-      <c r="C67" s="19">
+      <c r="C67" s="8">
         <v>45199</v>
       </c>
-      <c r="D67" s="16" t="s">
+      <c r="D67" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E67" s="17">
+      <c r="E67" s="16">
         <v>101533500</v>
       </c>
     </row>
     <row r="68" spans="2:5">
-      <c r="B68" s="19">
+      <c r="B68" s="8">
         <v>45200</v>
       </c>
-      <c r="C68" s="19">
+      <c r="C68" s="8">
         <v>45213</v>
       </c>
-      <c r="D68" s="16" t="s">
+      <c r="D68" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E68" s="17">
+      <c r="E68" s="16">
         <v>21710200</v>
       </c>
     </row>
     <row r="69" spans="2:5">
-      <c r="B69" s="19">
+      <c r="B69" s="8">
         <v>45200</v>
       </c>
-      <c r="C69" s="19">
+      <c r="C69" s="8">
         <v>45213</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="D69" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E69" s="17">
+      <c r="E69" s="16">
         <v>58555500</v>
       </c>
     </row>
     <row r="70" spans="2:5">
-      <c r="B70" s="19">
+      <c r="B70" s="8">
         <v>45200</v>
       </c>
-      <c r="C70" s="19">
+      <c r="C70" s="8">
         <v>45213</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="D70" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E70" s="17">
+      <c r="E70" s="16">
         <v>80944575</v>
       </c>
     </row>
     <row r="71" spans="2:5">
-      <c r="B71" s="19">
+      <c r="B71" s="8">
         <v>45200</v>
       </c>
-      <c r="C71" s="19">
+      <c r="C71" s="8">
         <v>45213</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="D71" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E71" s="17">
+      <c r="E71" s="16">
         <v>92418750</v>
       </c>
     </row>
     <row r="72" spans="2:5">
-      <c r="B72" s="19">
+      <c r="B72" s="8">
         <v>45214</v>
       </c>
-      <c r="C72" s="19">
+      <c r="C72" s="8">
         <v>45227</v>
       </c>
-      <c r="D72" s="16" t="s">
+      <c r="D72" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E72" s="17">
+      <c r="E72" s="16">
         <v>21382400</v>
       </c>
     </row>
     <row r="73" spans="2:5">
-      <c r="B73" s="19">
+      <c r="B73" s="8">
         <v>45214</v>
       </c>
-      <c r="C73" s="19">
+      <c r="C73" s="8">
         <v>45227</v>
       </c>
-      <c r="D73" s="16" t="s">
+      <c r="D73" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E73" s="17">
+      <c r="E73" s="16">
         <v>58796775</v>
       </c>
     </row>
     <row r="74" spans="2:5">
-      <c r="B74" s="19">
+      <c r="B74" s="8">
         <v>45214</v>
       </c>
-      <c r="C74" s="19">
+      <c r="C74" s="8">
         <v>45227</v>
       </c>
-      <c r="D74" s="16" t="s">
+      <c r="D74" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="17">
+      <c r="E74" s="16">
         <v>78798550</v>
       </c>
     </row>
     <row r="75" spans="2:5">
-      <c r="B75" s="19">
+      <c r="B75" s="8">
         <v>45214</v>
       </c>
-      <c r="C75" s="19">
+      <c r="C75" s="8">
         <v>45227</v>
       </c>
-      <c r="D75" s="16" t="s">
+      <c r="D75" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E75" s="17">
+      <c r="E75" s="16">
         <v>91655250</v>
       </c>
     </row>
     <row r="76" spans="2:5">
-      <c r="B76" s="19">
+      <c r="B76" s="8">
         <v>45228</v>
       </c>
-      <c r="C76" s="19">
+      <c r="C76" s="8">
         <v>45241</v>
       </c>
-      <c r="D76" s="16" t="s">
+      <c r="D76" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="17">
+      <c r="E76" s="16">
         <v>20081200</v>
       </c>
     </row>
     <row r="77" spans="2:5">
-      <c r="B77" s="19">
+      <c r="B77" s="8">
         <v>45228</v>
       </c>
-      <c r="C77" s="19">
+      <c r="C77" s="8">
         <v>45241</v>
       </c>
-      <c r="D77" s="16" t="s">
+      <c r="D77" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E77" s="17">
+      <c r="E77" s="16">
         <v>44149525</v>
       </c>
     </row>
     <row r="78" spans="2:5">
-      <c r="B78" s="19">
+      <c r="B78" s="8">
         <v>45228</v>
       </c>
-      <c r="C78" s="19">
+      <c r="C78" s="8">
         <v>45241</v>
       </c>
-      <c r="D78" s="16" t="s">
+      <c r="D78" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="17">
+      <c r="E78" s="16">
         <v>69366350</v>
       </c>
     </row>
     <row r="79" spans="2:5">
-      <c r="B79" s="19">
+      <c r="B79" s="8">
         <v>45228</v>
       </c>
-      <c r="C79" s="19">
+      <c r="C79" s="8">
         <v>45241</v>
       </c>
-      <c r="D79" s="16" t="s">
+      <c r="D79" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E79" s="17">
+      <c r="E79" s="16">
         <v>85588500</v>
       </c>
     </row>
@@ -5617,7 +5630,7 @@
   </sheetPr>
   <dimension ref="A3:B132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A7" sqref="A7 A11:A12 A15:A16 A20:A21 A24:A25 A28:A29 A32:A33 A36:A37 A41:A42 A45:A46 A49:A53 A57:A62 A65:A71 A75:A80 A83:A86 A90:A93 A96:A99 A103:A106 A109:A112 A116:A119 A122:A125 A128:A131"/>
       <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" activeRow="23" previousRow="23" click="1" r:id="rId1">
         <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
@@ -6695,19 +6708,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="13.8571428571429" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.8571428571429" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.8571428571429" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.8571428571429" style="4" customWidth="1"/>
     <col min="4" max="4" width="29.8571428571429" customWidth="1"/>
-    <col min="5" max="5" width="16.8571428571429" style="2"/>
+    <col min="5" max="5" width="16.8571428571429" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="3" spans="2:5">
       <c r="B3" s="6" t="s">
@@ -6733,7 +6746,7 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>53207688</v>
       </c>
     </row>
@@ -6747,7 +6760,7 @@
       <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="5">
         <v>166175019</v>
       </c>
     </row>
@@ -6761,7 +6774,7 @@
       <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <v>800282862</v>
       </c>
     </row>
@@ -6775,7 +6788,7 @@
       <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="5">
         <v>30173067</v>
       </c>
     </row>
@@ -6783,13 +6796,13 @@
       <c r="B8" s="8">
         <v>45056</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <v>3415000</v>
       </c>
     </row>
@@ -6803,7 +6816,7 @@
       <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="5">
         <v>234976006</v>
       </c>
     </row>
@@ -6817,7 +6830,7 @@
       <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="5">
         <v>3546410</v>
       </c>
     </row>
@@ -6831,7 +6844,7 @@
       <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="5">
         <v>304242133</v>
       </c>
     </row>
@@ -6845,7 +6858,7 @@
       <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="5">
         <v>5263910</v>
       </c>
     </row>
@@ -6859,7 +6872,7 @@
       <c r="D13" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="5">
         <v>363521956</v>
       </c>
     </row>
@@ -6873,7 +6886,7 @@
       <c r="D14" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="5">
         <v>350394068</v>
       </c>
     </row>
@@ -6887,7 +6900,7 @@
       <c r="D15" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="5">
         <v>404476960</v>
       </c>
     </row>
@@ -6901,7 +6914,7 @@
       <c r="D16" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="5">
         <v>400932654</v>
       </c>
     </row>
@@ -6915,7 +6928,7 @@
       <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="5">
         <v>10850000</v>
       </c>
     </row>
@@ -6929,7 +6942,7 @@
       <c r="D18" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="5">
         <v>14112500</v>
       </c>
     </row>
@@ -6943,7 +6956,7 @@
       <c r="D19" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="5">
         <v>5715000</v>
       </c>
     </row>
@@ -6957,7 +6970,7 @@
       <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="5">
         <v>13497500</v>
       </c>
     </row>
@@ -6971,7 +6984,7 @@
       <c r="D21" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="5">
         <v>24010250</v>
       </c>
     </row>
@@ -6985,7 +6998,7 @@
       <c r="D22" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="5">
         <v>21612500</v>
       </c>
     </row>
@@ -6999,7 +7012,7 @@
       <c r="D23" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="5">
         <v>3677235</v>
       </c>
     </row>
@@ -7013,7 +7026,7 @@
       <c r="D24" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="5">
         <v>26861772</v>
       </c>
     </row>
@@ -7027,7 +7040,7 @@
       <c r="D25" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="5">
         <v>25270572</v>
       </c>
     </row>
@@ -7041,7 +7054,7 @@
       <c r="D26" t="s">
         <v>49</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="5">
         <v>26589262</v>
       </c>
     </row>
@@ -7055,7 +7068,7 @@
       <c r="D27" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="5">
         <v>26497488</v>
       </c>
     </row>
@@ -7069,4 +7082,74 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="C4:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="3" max="3" width="42.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:4">
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4">
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="3:4">
+      <c r="C6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="3:4">
+      <c r="C7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="3:4">
+      <c r="C8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="3:4">
+      <c r="C9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="3:4">
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="3:4">
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>